<commit_message>
Add ID in all data
</commit_message>
<xml_diff>
--- a/data/excel/other_words.xlsx
+++ b/data/excel/other_words.xlsx
@@ -13,8 +13,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Tiempo)" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ARTÍCULOS (Artículos y determin" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONJUNCIONES (Conjunciones)" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBRES (Pronombres)" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBROS (Pronombres)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categoría" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBRES (Pronombres)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBROS (Pronombres)" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,20 +444,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -465,362 +471,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13020</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>always</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ól-weis</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>siempre</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13021</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>usually</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>jú-ual-li</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>usualmente</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>often</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>óf-en</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>a menudo</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>sometimes</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>sám-taims</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>a veces</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>rarely</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>rér-li</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>poco frecuentemente</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>never</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>né-ver</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>nunca</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13026</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>daily</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>deil-i</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>diariamente</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13027</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>weekly</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>wi-kli</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>semanalmente</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13028</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>monthly</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>mán-thli</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>mensualmente</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13029</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>annually</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>án-nu-al-li</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>anualmente</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13030</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>occasionally</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>okéi-sho-nal-li</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>ocasionalmente</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13031</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>frequently</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>frí-kwent-li</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>frecuntemente</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>frecuentemente</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13032</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>constantly</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>kón-stant-li</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>constantemente</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13033</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>regularly</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>ré-gu-lar-li</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>regularmente</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13034</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>hardly</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>há-dli</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>dificilmente</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13035</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>seldom</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>sél-dum</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>rara vez</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13036</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>intermittently</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>in-tér-mí-ten-tli</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>intermitentemente</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13037</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>repeatedly</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>ri-pí-ted-li</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repetidamente</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>repetidamente</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13038</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>every day</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>év-ri deí</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>cada día</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13039</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>once</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>uan</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>una vez</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -833,7 +939,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,20 +950,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -866,362 +977,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13040</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>here</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>híer</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>aquí</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13041</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>there</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>ðér</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>allí</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13042</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>everywhere</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>év-ri-uér</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>todo lugar</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13043</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>somewhere</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>sám-uer</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>lugar desconocido</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13044</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>nowhere</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>nóu-uer</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>en ninguna parte</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13045</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>above</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>abáv</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>encima</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13046</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>below</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>bilóu</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>debajo</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13047</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>inside</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>ín-said</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>adentro</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13048</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>outside</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>áut-said</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>afuera</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13049</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>upstairs</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>ap-sterz</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>arriba</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13050</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>downstairs</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>daún-sterz</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>abajo</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13051</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>forward</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>fór-ward</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>hacia adelante</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13052</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>backward</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>bák-wérd</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>hacia atrás</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13053</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>ahead</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>a-jéd</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>delante</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13054</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>behind</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>bi-háind</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>atrás</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13055</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>nearby</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>nír-bai</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>cerca</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13056</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>far</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>fár</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>lejos</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13057</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>away</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>awéi</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>lejos</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13058</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>around</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>ar-áund</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>alrededor</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13059</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>between</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>bi-twín</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>entre</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1234,7 +1445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1245,20 +1456,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -1267,362 +1483,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13060</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>quickly</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>kwik-li</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>rápidamente</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13061</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>slowly</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>slóu-li</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>despacio</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13062</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>well</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>uel</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>bien</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13063</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>badly</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>bád-li</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>mal</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13064</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>easily</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>íz-ili</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>fácilmente</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13065</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>hardly</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>há-dli</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>dificilmente</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13066</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>carefully</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>kér-fu-li</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>cuidadosamente</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13067</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>carelessly</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>kér-les-li</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>descuidadamente</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13068</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>quietly</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>kwáit-li</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>silenciosamente</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13069</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>loudly</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>láud-li</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>ruidosamente</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13070</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>strongly</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>stróng-li</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>fuerzudamente</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13071</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>weakly</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>wí-klí</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>debilmente</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13072</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>clearly</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>klír-li</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>claramente</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13073</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>roughly</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>róf-li</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>bruscamente</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13074</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>softly</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>sof-li</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>suavemente</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13075</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>deeply</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>dí-pli</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>profundamente</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13076</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>highly</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>jái-li</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>en gran medida</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13077</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>extremely</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>iks-trí-mli</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>extremadamente</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13078</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>totally</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>tóu-tali</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>totalmente</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13079</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>barely</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>bér-li</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>apenas</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1635,7 +1951,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1646,20 +1962,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -1668,362 +1989,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13000</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>now</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>nau</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>ahora</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>then</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>ðen</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>luego</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13002</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>today</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>tudéi</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>hoy</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>tomorrow</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>tomó-rou</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>mañana</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13004</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>yesterday</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>yé-ster-déi</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>ayer</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13005</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>soon</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>sun</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>pronto</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13006</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>later</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>léi-ter</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>luego</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13007</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>early</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>ér-li</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>temprano</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13008</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>late</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>leít</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>tarde</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13009</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>already</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>ól-red-i</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>ya</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13010</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>still</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>stíl</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>aún</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13011</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>yet</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>yet</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>aún</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13012</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>just</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>just</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>justo</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13013</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>finally</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>fáin-al-li</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>finalmente</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13014</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>recently</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>rís-nt-li</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>recientemente</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13015</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>always</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>ól-weis</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>siempre</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13016</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>never</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>né-ver</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>nunca</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13017</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>ever</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>é-ver</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>alguna vez</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13018</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>often</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>óf-en</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>a menudo</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13019</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>sometimes</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>sám-taims</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>a veces</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2036,7 +2457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,20 +2468,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -2069,362 +2495,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13100</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>the</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ðe</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>el/la</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13101</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>a</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>eiy</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>un/una</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13102</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>an</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>án</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>un/una</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13103</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>some</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>sam</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>algunos</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13104</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>any</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>éni</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>cualquier</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13105</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>this</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>ðis</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>este/esta</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13106</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>that</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>ðat</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>ese/esa</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13107</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>these</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>ðíz</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>estos/estas</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13108</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>those</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>ðóus</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>esos/esas</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13109</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>my</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>mai</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>mi</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13110</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>your</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>iór</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>tuyo/a</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13111</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>his</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>híz</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>suyo</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13112</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>her</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>hér</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>suya</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13113</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>its</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>its</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>suyo</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13114</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>our</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>áur</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>nuestro</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13115</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>their</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>ðeir</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>suyo</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13116</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>few</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>fiú</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>pocos</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13117</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>many</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>méni</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> muchos</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>muchos</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13118</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>much</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>múch</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>mucho</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13119</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>nó</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>ninguno</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2437,7 +2963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2448,20 +2974,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -2470,362 +3001,462 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13080</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>and</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ánd</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>13081</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>but</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>bat</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>pero</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13082</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>or</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>ór</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>o</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>13083</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>so</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>sou</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>así que</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>13084</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>because</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>bikóz</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>porque</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>13085</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>although</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>ól-dóu</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> aunque</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>aunque</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>13086</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>if</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>íf</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>13087</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>when</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>juén</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>cuando</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>13088</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>while</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>juáíl</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>mientras</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>13089</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>before</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>bifór</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>antes</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>13090</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>after</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>áfter</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>después</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>13091</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>since</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>sins</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>desde</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>13092</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>until</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>án-til</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>hasta</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>13093</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>unless</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>án-les</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> a menos que</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>a menos que</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>13094</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>whereas</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>hué-re-az</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>mientras que</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>13095</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>as</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>az</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>como</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>13096</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>though</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>ðou</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> aunque</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>aunque</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>13097</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>even if</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>í-vn if</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>aún si</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>13098</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>even though</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>í-vn ðou</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>aunque</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>13099</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>whether</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>ué-ðer</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2838,7 +3469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2849,20 +3480,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -2871,344 +3507,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ái</t>
+          <t>Palabra en Inglés</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>yo</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>you</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>iu</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>tú</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>he</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ji</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>él</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>she</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>shí</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ella</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>it</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>it</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>eso</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>we</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>wí</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> nosotros/as</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>they</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ðéi</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ellos/as</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>me</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>mí</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>a mí</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>him</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>hím</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>a él</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>her</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>hér</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>a ella</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>us</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ás</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>a nosotros</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>them</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ðem</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>a ellos</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>mine</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>main</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>mío</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>yours</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>iórs</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>tuyo/a</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>his</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>híz</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>suyo</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>hers</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>hérs</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>suyo/a</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ours</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>áurs</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nuestro</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>theirs</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>ðéers</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>suyo</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>myself</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>maíf-self</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>yo mismo/a</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>Pronunciación</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Traducción</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3221,7 +3538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3232,20 +3549,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Inglés</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Pronunciación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Traducción</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Visualización</t>
         </is>
@@ -3254,20 +3576,508 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>13120</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ái</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>yo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>13121</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>you</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>tú</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13122</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>he</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ji</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>él</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13123</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>she</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>shí</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ella</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13124</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>eso</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13125</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>we</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>wí</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nosotros/as</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13126</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>they</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ðéi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ellos/as</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13127</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>mí</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>a mí</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>13128</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>him</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>hím</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>a él</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>13129</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>her</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>hér</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>a ella</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>13130</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>us</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ás</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>a nosotros</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>13131</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>them</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ðem</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>a ellos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13132</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mine</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>mío</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13133</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>yours</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>iórs</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>tuyo/a</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>13134</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>his</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>híz</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>suyo</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>13135</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>hers</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>hérs</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>suyo/a</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>13136</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ours</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>áurs</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nuestro</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>13137</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>theirs</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ðéers</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>suyo</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>13138</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>myself</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>maíf-self</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>yo mismo/a</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inglés</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Pronunciación</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Traducción</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>13139</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>yourself</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>iór-self</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>tú mismo/a</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ordened data for ID
</commit_message>
<xml_diff>
--- a/data/excel/other_words.xlsx
+++ b/data/excel/other_words.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Frecuencia)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Lugar y dirección)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Modo y grado)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Tiempo)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ARTÍCULOS (Artículos y determin" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONJUNCIONES (Conjunciones)" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categoría" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBRES (Pronombres)" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBROS (Pronombres)" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Tiempo)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Frecuencia)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Lugar y dirección)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADVERBIOS (Modo y grado)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONJUNCIONES (Conjunciones)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ARTÍCULOS (Artículos y determin" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBRES (Pronombres)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRONOMBROS (Pronombres)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categoría" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,22 +471,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13020</t>
+          <t>13000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>now</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ól-weis</t>
+          <t>nau</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>siempre</t>
+          <t>ahora</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -494,22 +494,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13021</t>
+          <t>13001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>usually</t>
+          <t>then</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>jú-ual-li</t>
+          <t>ðen</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>usualmente</t>
+          <t>luego</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -517,22 +517,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13022</t>
+          <t>13002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>often</t>
+          <t>today</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>óf-en</t>
+          <t>tudéi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>a menudo</t>
+          <t>hoy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -540,22 +540,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13023</t>
+          <t>13003</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sometimes</t>
+          <t>tomorrow</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sám-taims</t>
+          <t>tomó-rou</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>a veces</t>
+          <t>mañana</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -563,22 +563,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13024</t>
+          <t>13004</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>rarely</t>
+          <t>yesterday</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>rér-li</t>
+          <t>yé-ster-déi</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>poco frecuentemente</t>
+          <t>ayer</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -586,22 +586,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13025</t>
+          <t>13005</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>never</t>
+          <t>soon</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>né-ver</t>
+          <t>sun</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>nunca</t>
+          <t>pronto</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -609,22 +609,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13026</t>
+          <t>13006</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>daily</t>
+          <t>later</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>deil-i</t>
+          <t>léi-ter</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>diariamente</t>
+          <t>luego</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -632,22 +632,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13027</t>
+          <t>13007</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>weekly</t>
+          <t>early</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>wi-kli</t>
+          <t>ér-li</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>semanalmente</t>
+          <t>temprano</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -655,22 +655,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13028</t>
+          <t>13008</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>late</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>mán-thli</t>
+          <t>leít</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>mensualmente</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -678,22 +678,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13029</t>
+          <t>13009</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>annually</t>
+          <t>already</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>án-nu-al-li</t>
+          <t>ól-red-i</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>anualmente</t>
+          <t>ya</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -701,22 +701,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13030</t>
+          <t>13010</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>occasionally</t>
+          <t>still</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>okéi-sho-nal-li</t>
+          <t>stíl</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ocasionalmente</t>
+          <t>aún</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -724,22 +724,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13031</t>
+          <t>13011</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>frequently</t>
+          <t>yet</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>frí-kwent-li</t>
+          <t>yet</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>frecuentemente</t>
+          <t>aún</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -747,22 +747,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13032</t>
+          <t>13012</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>constantly</t>
+          <t>just</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>kón-stant-li</t>
+          <t>just</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>constantemente</t>
+          <t>justo</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -770,22 +770,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13033</t>
+          <t>13013</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>regularly</t>
+          <t>finally</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ré-gu-lar-li</t>
+          <t>fáin-al-li</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>regularmente</t>
+          <t>finalmente</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -793,22 +793,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13034</t>
+          <t>13014</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>hardly</t>
+          <t>recently</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>há-dli</t>
+          <t>rís-nt-li</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>dificilmente</t>
+          <t>recientemente</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -816,22 +816,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13035</t>
+          <t>13015</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>seldom</t>
+          <t>always</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>sél-dum</t>
+          <t>ól-weis</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>rara vez</t>
+          <t>siempre</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -839,22 +839,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13036</t>
+          <t>13016</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>intermittently</t>
+          <t>never</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>in-tér-mí-ten-tli</t>
+          <t>né-ver</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>intermitentemente</t>
+          <t>nunca</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -862,22 +862,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13037</t>
+          <t>13017</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>repeatedly</t>
+          <t>ever</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ri-pí-ted-li</t>
+          <t>é-ver</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>repetidamente</t>
+          <t>alguna vez</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -885,22 +885,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13038</t>
+          <t>13018</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>every day</t>
+          <t>often</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>év-ri deí</t>
+          <t>óf-en</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>cada día</t>
+          <t>a menudo</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -908,22 +908,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13039</t>
+          <t>13019</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>once</t>
+          <t>sometimes</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>uan</t>
+          <t>sám-taims</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>una vez</t>
+          <t>a veces</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -977,22 +977,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13040</t>
+          <t>13020</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>here</t>
+          <t>always</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>híer</t>
+          <t>ól-weis</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>aquí</t>
+          <t>siempre</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1000,22 +1000,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13041</t>
+          <t>13021</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>there</t>
+          <t>usually</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ðér</t>
+          <t>jú-ual-li</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>allí</t>
+          <t>usualmente</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1023,22 +1023,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13042</t>
+          <t>13022</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>everywhere</t>
+          <t>often</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>év-ri-uér</t>
+          <t>óf-en</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>todo lugar</t>
+          <t>a menudo</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1046,22 +1046,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13043</t>
+          <t>13023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>somewhere</t>
+          <t>sometimes</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sám-uer</t>
+          <t>sám-taims</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>lugar desconocido</t>
+          <t>a veces</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1069,22 +1069,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13044</t>
+          <t>13024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>nowhere</t>
+          <t>rarely</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>nóu-uer</t>
+          <t>rér-li</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>en ninguna parte</t>
+          <t>poco frecuentemente</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1092,22 +1092,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13045</t>
+          <t>13025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>above</t>
+          <t>never</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>abáv</t>
+          <t>né-ver</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>encima</t>
+          <t>nunca</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1115,22 +1115,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13046</t>
+          <t>13026</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>below</t>
+          <t>daily</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>bilóu</t>
+          <t>deil-i</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>debajo</t>
+          <t>diariamente</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1138,22 +1138,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13047</t>
+          <t>13027</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>inside</t>
+          <t>weekly</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ín-said</t>
+          <t>wi-kli</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>adentro</t>
+          <t>semanalmente</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -1161,22 +1161,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13048</t>
+          <t>13028</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>outside</t>
+          <t>monthly</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>áut-said</t>
+          <t>mán-thli</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>afuera</t>
+          <t>mensualmente</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -1184,22 +1184,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13049</t>
+          <t>13029</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>upstairs</t>
+          <t>annually</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ap-sterz</t>
+          <t>án-nu-al-li</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>arriba</t>
+          <t>anualmente</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -1207,22 +1207,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13050</t>
+          <t>13030</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>downstairs</t>
+          <t>occasionally</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>daún-sterz</t>
+          <t>okéi-sho-nal-li</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>abajo</t>
+          <t>ocasionalmente</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -1230,22 +1230,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13051</t>
+          <t>13031</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>frequently</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fór-ward</t>
+          <t>frí-kwent-li</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>hacia adelante</t>
+          <t>frecuentemente</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1253,22 +1253,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13052</t>
+          <t>13032</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>backward</t>
+          <t>constantly</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>bák-wérd</t>
+          <t>kón-stant-li</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>hacia atrás</t>
+          <t>constantemente</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -1276,22 +1276,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13053</t>
+          <t>13033</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ahead</t>
+          <t>regularly</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>a-jéd</t>
+          <t>ré-gu-lar-li</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>delante</t>
+          <t>regularmente</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1299,22 +1299,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13054</t>
+          <t>13034</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>behind</t>
+          <t>hardly</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>bi-háind</t>
+          <t>há-dli</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>atrás</t>
+          <t>dificilmente</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1322,22 +1322,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13055</t>
+          <t>13035</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>nearby</t>
+          <t>seldom</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>nír-bai</t>
+          <t>sél-dum</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>cerca</t>
+          <t>rara vez</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1345,22 +1345,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13056</t>
+          <t>13036</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>far</t>
+          <t>intermittently</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fár</t>
+          <t>in-tér-mí-ten-tli</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>lejos</t>
+          <t>intermitentemente</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1368,22 +1368,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13057</t>
+          <t>13037</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>away</t>
+          <t>repeatedly</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>awéi</t>
+          <t>ri-pí-ted-li</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>lejos</t>
+          <t>repetidamente</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1391,22 +1391,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13058</t>
+          <t>13038</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>around</t>
+          <t>every day</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ar-áund</t>
+          <t>év-ri deí</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>alrededor</t>
+          <t>cada día</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1414,22 +1414,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13059</t>
+          <t>13039</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>between</t>
+          <t>once</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>bi-twín</t>
+          <t>uan</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>entre</t>
+          <t>una vez</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1483,22 +1483,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13060</t>
+          <t>13040</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>quickly</t>
+          <t>here</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>kwik-li</t>
+          <t>híer</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>rápidamente</t>
+          <t>aquí</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1506,22 +1506,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13061</t>
+          <t>13041</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>slowly</t>
+          <t>there</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>slóu-li</t>
+          <t>ðér</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>despacio</t>
+          <t>allí</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1529,22 +1529,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13062</t>
+          <t>13042</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>well</t>
+          <t>everywhere</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>uel</t>
+          <t>év-ri-uér</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>bien</t>
+          <t>todo lugar</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1552,22 +1552,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13063</t>
+          <t>13043</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>badly</t>
+          <t>somewhere</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>bád-li</t>
+          <t>sám-uer</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>mal</t>
+          <t>lugar desconocido</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1575,22 +1575,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13064</t>
+          <t>13044</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>easily</t>
+          <t>nowhere</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>íz-ili</t>
+          <t>nóu-uer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>fácilmente</t>
+          <t>en ninguna parte</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1598,22 +1598,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13065</t>
+          <t>13045</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>hardly</t>
+          <t>above</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>há-dli</t>
+          <t>abáv</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>dificilmente</t>
+          <t>encima</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1621,22 +1621,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13066</t>
+          <t>13046</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>carefully</t>
+          <t>below</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>kér-fu-li</t>
+          <t>bilóu</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>cuidadosamente</t>
+          <t>debajo</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1644,22 +1644,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13067</t>
+          <t>13047</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>carelessly</t>
+          <t>inside</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>kér-les-li</t>
+          <t>ín-said</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>descuidadamente</t>
+          <t>adentro</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -1667,22 +1667,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13068</t>
+          <t>13048</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>quietly</t>
+          <t>outside</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>kwáit-li</t>
+          <t>áut-said</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>silenciosamente</t>
+          <t>afuera</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -1690,22 +1690,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13069</t>
+          <t>13049</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>loudly</t>
+          <t>upstairs</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>láud-li</t>
+          <t>ap-sterz</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ruidosamente</t>
+          <t>arriba</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -1713,22 +1713,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13070</t>
+          <t>13050</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>strongly</t>
+          <t>downstairs</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>stróng-li</t>
+          <t>daún-sterz</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>fuerzudamente</t>
+          <t>abajo</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -1736,22 +1736,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13071</t>
+          <t>13051</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>weakly</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>wí-klí</t>
+          <t>fór-ward</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>debilmente</t>
+          <t>hacia adelante</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1759,22 +1759,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13072</t>
+          <t>13052</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>clearly</t>
+          <t>backward</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>klír-li</t>
+          <t>bák-wérd</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>claramente</t>
+          <t>hacia atrás</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -1782,22 +1782,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13073</t>
+          <t>13053</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>roughly</t>
+          <t>ahead</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>róf-li</t>
+          <t>a-jéd</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>bruscamente</t>
+          <t>delante</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1805,22 +1805,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13074</t>
+          <t>13054</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>softly</t>
+          <t>behind</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>sof-li</t>
+          <t>bi-háind</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>suavemente</t>
+          <t>atrás</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1828,22 +1828,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13075</t>
+          <t>13055</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>deeply</t>
+          <t>nearby</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dí-pli</t>
+          <t>nír-bai</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>profundamente</t>
+          <t>cerca</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1851,22 +1851,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13076</t>
+          <t>13056</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>highly</t>
+          <t>far</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>jái-li</t>
+          <t>fár</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>en gran medida</t>
+          <t>lejos</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1874,22 +1874,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13077</t>
+          <t>13057</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>extremely</t>
+          <t>away</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>iks-trí-mli</t>
+          <t>awéi</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>extremadamente</t>
+          <t>lejos</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1897,22 +1897,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13078</t>
+          <t>13058</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>totally</t>
+          <t>around</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>tóu-tali</t>
+          <t>ar-áund</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>totalmente</t>
+          <t>alrededor</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1920,22 +1920,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13079</t>
+          <t>13059</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>barely</t>
+          <t>between</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>bér-li</t>
+          <t>bi-twín</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>apenas</t>
+          <t>entre</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1989,22 +1989,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13000</t>
+          <t>13060</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>now</t>
+          <t>quickly</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>nau</t>
+          <t>kwik-li</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ahora</t>
+          <t>rápidamente</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -2012,22 +2012,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13001</t>
+          <t>13061</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>then</t>
+          <t>slowly</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ðen</t>
+          <t>slóu-li</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>luego</t>
+          <t>despacio</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -2035,22 +2035,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13002</t>
+          <t>13062</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>today</t>
+          <t>well</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>tudéi</t>
+          <t>uel</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>hoy</t>
+          <t>bien</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -2058,22 +2058,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13003</t>
+          <t>13063</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>tomorrow</t>
+          <t>badly</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>tomó-rou</t>
+          <t>bád-li</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>mañana</t>
+          <t>mal</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -2081,22 +2081,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13004</t>
+          <t>13064</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>yesterday</t>
+          <t>easily</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>yé-ster-déi</t>
+          <t>íz-ili</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ayer</t>
+          <t>fácilmente</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -2104,22 +2104,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13005</t>
+          <t>13065</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>soon</t>
+          <t>hardly</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sun</t>
+          <t>há-dli</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>pronto</t>
+          <t>dificilmente</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -2127,22 +2127,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13006</t>
+          <t>13066</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>later</t>
+          <t>carefully</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>léi-ter</t>
+          <t>kér-fu-li</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>luego</t>
+          <t>cuidadosamente</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -2150,22 +2150,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13007</t>
+          <t>13067</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>early</t>
+          <t>carelessly</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ér-li</t>
+          <t>kér-les-li</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>temprano</t>
+          <t>descuidadamente</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2173,22 +2173,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13008</t>
+          <t>13068</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>late</t>
+          <t>quietly</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>leít</t>
+          <t>kwáit-li</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>tarde</t>
+          <t>silenciosamente</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2196,22 +2196,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13009</t>
+          <t>13069</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>already</t>
+          <t>loudly</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ól-red-i</t>
+          <t>láud-li</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ya</t>
+          <t>ruidosamente</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2219,22 +2219,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13010</t>
+          <t>13070</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>still</t>
+          <t>strongly</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>stíl</t>
+          <t>stróng-li</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>aún</t>
+          <t>fuerzudamente</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2242,22 +2242,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13011</t>
+          <t>13071</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>yet</t>
+          <t>weakly</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>yet</t>
+          <t>wí-klí</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>aún</t>
+          <t>debilmente</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2265,22 +2265,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13012</t>
+          <t>13072</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>just</t>
+          <t>clearly</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>just</t>
+          <t>klír-li</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>justo</t>
+          <t>claramente</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -2288,22 +2288,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13013</t>
+          <t>13073</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>finally</t>
+          <t>roughly</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fáin-al-li</t>
+          <t>róf-li</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>finalmente</t>
+          <t>bruscamente</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -2311,22 +2311,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13014</t>
+          <t>13074</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>recently</t>
+          <t>softly</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>rís-nt-li</t>
+          <t>sof-li</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>recientemente</t>
+          <t>suavemente</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -2334,22 +2334,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13015</t>
+          <t>13075</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>deeply</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ól-weis</t>
+          <t>dí-pli</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>siempre</t>
+          <t>profundamente</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -2357,22 +2357,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13016</t>
+          <t>13076</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>never</t>
+          <t>highly</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>né-ver</t>
+          <t>jái-li</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>nunca</t>
+          <t>en gran medida</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -2380,22 +2380,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13017</t>
+          <t>13077</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ever</t>
+          <t>extremely</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>é-ver</t>
+          <t>iks-trí-mli</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>alguna vez</t>
+          <t>extremadamente</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -2403,22 +2403,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13018</t>
+          <t>13078</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>often</t>
+          <t>totally</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>óf-en</t>
+          <t>tóu-tali</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>a menudo</t>
+          <t>totalmente</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -2426,22 +2426,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13019</t>
+          <t>13079</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>sometimes</t>
+          <t>barely</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>sám-taims</t>
+          <t>bér-li</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>a veces</t>
+          <t>apenas</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -2495,22 +2495,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13100</t>
+          <t>13080</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>the</t>
+          <t>and</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ðe</t>
+          <t>ánd</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>el/la</t>
+          <t>y</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -2518,22 +2518,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13101</t>
+          <t>13081</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>but</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>eiy</t>
+          <t>bat</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>un/una</t>
+          <t>pero</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -2541,22 +2541,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13102</t>
+          <t>13082</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>an</t>
+          <t>or</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>án</t>
+          <t>ór</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>un/una</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -2564,22 +2564,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13103</t>
+          <t>13083</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>some</t>
+          <t>so</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sam</t>
+          <t>sou</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>algunos</t>
+          <t>así que</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -2587,22 +2587,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13104</t>
+          <t>13084</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>any</t>
+          <t>because</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>éni</t>
+          <t>bikóz</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>cualquier</t>
+          <t>porque</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -2610,22 +2610,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13105</t>
+          <t>13085</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>this</t>
+          <t>although</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ðis</t>
+          <t>ól-dóu</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>este/esta</t>
+          <t>aunque</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -2633,22 +2633,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13106</t>
+          <t>13086</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>that</t>
+          <t>if</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ðat</t>
+          <t>íf</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ese/esa</t>
+          <t>si</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -2656,22 +2656,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13107</t>
+          <t>13087</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>these</t>
+          <t>when</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ðíz</t>
+          <t>juén</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>estos/estas</t>
+          <t>cuando</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2679,22 +2679,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13108</t>
+          <t>13088</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>those</t>
+          <t>while</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ðóus</t>
+          <t>juáíl</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>esos/esas</t>
+          <t>mientras</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2702,22 +2702,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13109</t>
+          <t>13089</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>my</t>
+          <t>before</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>mai</t>
+          <t>bifór</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>mi</t>
+          <t>antes</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2725,22 +2725,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13110</t>
+          <t>13090</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>your</t>
+          <t>after</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>iór</t>
+          <t>áfter</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>tuyo/a</t>
+          <t>después</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2748,22 +2748,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13111</t>
+          <t>13091</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>his</t>
+          <t>since</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>híz</t>
+          <t>sins</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>suyo</t>
+          <t>desde</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2771,22 +2771,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13112</t>
+          <t>13092</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>her</t>
+          <t>until</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>hér</t>
+          <t>án-til</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>suya</t>
+          <t>hasta</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -2794,22 +2794,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13113</t>
+          <t>13093</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>its</t>
+          <t>unless</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>its</t>
+          <t>án-les</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>suyo</t>
+          <t>a menos que</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -2817,22 +2817,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13114</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>our</t>
+          <t>whereas</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>áur</t>
+          <t>hué-re-az</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>nuestro</t>
+          <t>mientras que</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -2840,22 +2840,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13115</t>
+          <t>13095</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>their</t>
+          <t>as</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ðeir</t>
+          <t>az</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>suyo</t>
+          <t>como</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -2863,22 +2863,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13116</t>
+          <t>13096</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>few</t>
+          <t>though</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fiú</t>
+          <t>ðou</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>pocos</t>
+          <t>aunque</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -2886,22 +2886,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13117</t>
+          <t>13097</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>many</t>
+          <t>even if</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>méni</t>
+          <t>í-vn if</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>muchos</t>
+          <t>aún si</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -2909,22 +2909,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13118</t>
+          <t>13098</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>much</t>
+          <t>even though</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>múch</t>
+          <t>í-vn ðou</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>mucho</t>
+          <t>aunque</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -2932,22 +2932,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13119</t>
+          <t>13099</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>whether</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>nó</t>
+          <t>ué-ðer</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ninguno</t>
+          <t>si</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -3001,22 +3001,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13080</t>
+          <t>13100</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>and</t>
+          <t>the</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ánd</t>
+          <t>ðe</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>el/la</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -3024,22 +3024,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13081</t>
+          <t>13101</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>but</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>bat</t>
+          <t>eiy</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pero</t>
+          <t>un/una</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -3047,22 +3047,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13082</t>
+          <t>13102</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>or</t>
+          <t>an</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ór</t>
+          <t>án</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>un/una</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -3070,22 +3070,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13083</t>
+          <t>13103</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>so</t>
+          <t>some</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sou</t>
+          <t>sam</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>así que</t>
+          <t>algunos</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -3093,22 +3093,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>13084</t>
+          <t>13104</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>because</t>
+          <t>any</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>bikóz</t>
+          <t>éni</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>porque</t>
+          <t>cualquier</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -3116,22 +3116,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13085</t>
+          <t>13105</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>although</t>
+          <t>this</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ól-dóu</t>
+          <t>ðis</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>aunque</t>
+          <t>este/esta</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -3139,22 +3139,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13086</t>
+          <t>13106</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>that</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>íf</t>
+          <t>ðat</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>ese/esa</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -3162,22 +3162,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13087</t>
+          <t>13107</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>when</t>
+          <t>these</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>juén</t>
+          <t>ðíz</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>cuando</t>
+          <t>estos/estas</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -3185,22 +3185,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13088</t>
+          <t>13108</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>while</t>
+          <t>those</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>juáíl</t>
+          <t>ðóus</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>mientras</t>
+          <t>esos/esas</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -3208,22 +3208,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13089</t>
+          <t>13109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>before</t>
+          <t>my</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>bifór</t>
+          <t>mai</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>antes</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -3231,22 +3231,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13090</t>
+          <t>13110</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>after</t>
+          <t>your</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>áfter</t>
+          <t>iór</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>después</t>
+          <t>tuyo/a</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -3254,22 +3254,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13091</t>
+          <t>13111</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>since</t>
+          <t>his</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>sins</t>
+          <t>híz</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>desde</t>
+          <t>suyo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -3277,22 +3277,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13092</t>
+          <t>13112</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>until</t>
+          <t>her</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>án-til</t>
+          <t>hér</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>hasta</t>
+          <t>suya</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3300,22 +3300,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>13093</t>
+          <t>13113</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>unless</t>
+          <t>its</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>án-les</t>
+          <t>its</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>a menos que</t>
+          <t>suyo</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3323,22 +3323,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>13114</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>whereas</t>
+          <t>our</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>hué-re-az</t>
+          <t>áur</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>mientras que</t>
+          <t>nuestro</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3346,22 +3346,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>13095</t>
+          <t>13115</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>as</t>
+          <t>their</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>az</t>
+          <t>ðeir</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>como</t>
+          <t>suyo</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3369,22 +3369,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13096</t>
+          <t>13116</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>though</t>
+          <t>few</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ðou</t>
+          <t>fiú</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>aunque</t>
+          <t>pocos</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3392,22 +3392,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13097</t>
+          <t>13117</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>even if</t>
+          <t>many</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>í-vn if</t>
+          <t>méni</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>aún si</t>
+          <t>muchos</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -3415,22 +3415,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13098</t>
+          <t>13118</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>even though</t>
+          <t>much</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>í-vn ðou</t>
+          <t>múch</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>aunque</t>
+          <t>mucho</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -3438,22 +3438,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13099</t>
+          <t>13119</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>whether</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ué-ðer</t>
+          <t>nó</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>ninguno</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -3464,6 +3464,489 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inglés</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Pronunciación</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Traducción</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Visualización</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>13120</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ái</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>yo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>13121</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>you</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>tú</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13122</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>he</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ji</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>él</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13123</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>she</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>shí</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ella</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13124</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>eso</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13125</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>we</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>wí</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nosotros/as</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13126</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>they</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ðéi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ellos/as</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13127</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>mí</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>a mí</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>13128</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>him</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>hím</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>a él</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>13129</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>her</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>hér</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>a ella</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>13130</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>us</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ás</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>a nosotros</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>13131</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>them</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ðem</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>a ellos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13132</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mine</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>mío</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13133</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>yours</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>iórs</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>tuyo/a</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>13134</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>his</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>híz</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>suyo</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>13135</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>hers</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>hérs</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>suyo/a</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>13136</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ours</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>áurs</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nuestro</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>13137</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>theirs</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ðéers</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>suyo</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>13138</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>myself</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>maíf-self</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>yo mismo/a</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3507,508 +3990,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>13139</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Palabra en Inglés</t>
+          <t>yourself</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pronunciación</t>
+          <t>iór-self</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Traducción</t>
+          <t>tú mismo/a</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Inglés</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Pronunciación</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Traducción</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Visualización</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>13120</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ái</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>yo</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>13121</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>you</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>iu</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>tú</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>13122</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>he</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ji</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>él</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>13123</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>she</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>shí</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ella</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>13124</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>it</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>it</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>eso</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>13125</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>we</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>wí</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>nosotros/as</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>13126</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>they</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ðéi</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ellos/as</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>13127</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>me</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>mí</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>a mí</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>13128</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>him</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>hím</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>a él</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>13129</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>her</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>hér</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>a ella</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>13130</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>us</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>ás</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>a nosotros</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>13131</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>them</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>ðem</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>a ellos</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13132</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>mine</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>main</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>mío</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>13133</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>yours</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>iórs</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>tuyo/a</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>13134</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>his</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>híz</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>suyo</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>13135</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>hers</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>hérs</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>suyo/a</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>13136</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>ours</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>áurs</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>nuestro</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>13137</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>theirs</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>ðéers</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>suyo</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>13138</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>myself</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>maíf-self</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>yo mismo/a</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4059,22 +4059,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13139</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>yourself</t>
+          <t>Palabra en Inglés</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iór-self</t>
+          <t>Pronunciación</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>tú mismo/a</t>
+          <t>Traducción</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>

</xml_diff>